<commit_message>
cambios 11 de marzo
</commit_message>
<xml_diff>
--- a/models/BD MCC.xlsx
+++ b/models/BD MCC.xlsx
@@ -2277,7 +2277,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F293"/>
+  <dimension ref="A1:F316"/>
   <sheetViews>
     <sheetView topLeftCell="A226" workbookViewId="0">
       <selection activeCell="B187" sqref="B187"/>
@@ -8820,6 +8820,443 @@
       </c>
       <c r="F293" t="n">
         <v>20</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>292</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Jorgito</t>
+        </is>
+      </c>
+      <c r="C294" t="n">
+        <v>0</v>
+      </c>
+      <c r="D294" t="n">
+        <v>34</v>
+      </c>
+      <c r="F294" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>PEREZ</t>
+        </is>
+      </c>
+      <c r="C295" t="n">
+        <v>1</v>
+      </c>
+      <c r="D295" t="n">
+        <v>34</v>
+      </c>
+      <c r="F295" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>PEREZ</t>
+        </is>
+      </c>
+      <c r="C296" t="n">
+        <v>1</v>
+      </c>
+      <c r="D296" t="n">
+        <v>34</v>
+      </c>
+      <c r="F296" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>PEREZ</t>
+        </is>
+      </c>
+      <c r="C297" t="n">
+        <v>1</v>
+      </c>
+      <c r="D297" t="n">
+        <v>34</v>
+      </c>
+      <c r="F297" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>JIJIJA</t>
+        </is>
+      </c>
+      <c r="C298" t="n">
+        <v>0</v>
+      </c>
+      <c r="D298" t="n">
+        <v>29</v>
+      </c>
+      <c r="F298" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>EEE</t>
+        </is>
+      </c>
+      <c r="C299" t="n">
+        <v>1</v>
+      </c>
+      <c r="D299" t="n">
+        <v>29</v>
+      </c>
+      <c r="F299" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>uuu</t>
+        </is>
+      </c>
+      <c r="C300" t="n">
+        <v>0</v>
+      </c>
+      <c r="D300" t="n">
+        <v>39</v>
+      </c>
+      <c r="F300" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>lineas</t>
+        </is>
+      </c>
+      <c r="C301" t="n">
+        <v>0</v>
+      </c>
+      <c r="D301" t="n">
+        <v>32</v>
+      </c>
+      <c r="F301" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>300</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>rene</t>
+        </is>
+      </c>
+      <c r="C302" t="n">
+        <v>0</v>
+      </c>
+      <c r="D302" t="n">
+        <v>23</v>
+      </c>
+      <c r="F302" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>angel</t>
+        </is>
+      </c>
+      <c r="C303" t="n">
+        <v>0</v>
+      </c>
+      <c r="D303" t="n">
+        <v>35</v>
+      </c>
+      <c r="F303" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>rodrigo</t>
+        </is>
+      </c>
+      <c r="C304" t="n">
+        <v>0</v>
+      </c>
+      <c r="D304" t="n">
+        <v>37</v>
+      </c>
+      <c r="F304" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Hola</t>
+        </is>
+      </c>
+      <c r="C305" t="n">
+        <v>0</v>
+      </c>
+      <c r="D305" t="n">
+        <v>23</v>
+      </c>
+      <c r="F305" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>olis</t>
+        </is>
+      </c>
+      <c r="C306" t="n">
+        <v>0</v>
+      </c>
+      <c r="D306" t="n">
+        <v>23</v>
+      </c>
+      <c r="F306" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>INDIRA</t>
+        </is>
+      </c>
+      <c r="C307" t="n">
+        <v>1</v>
+      </c>
+      <c r="D307" t="n">
+        <v>29</v>
+      </c>
+      <c r="F307" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>jejej</t>
+        </is>
+      </c>
+      <c r="C308" t="n">
+        <v>0</v>
+      </c>
+      <c r="D308" t="n">
+        <v>23</v>
+      </c>
+      <c r="F308" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Ma</t>
+        </is>
+      </c>
+      <c r="C309" t="n">
+        <v>0</v>
+      </c>
+      <c r="D309" t="n">
+        <v>25</v>
+      </c>
+      <c r="F309" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>ola</t>
+        </is>
+      </c>
+      <c r="C310" t="n">
+        <v>1</v>
+      </c>
+      <c r="D310" t="n">
+        <v>37</v>
+      </c>
+      <c r="F310" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Manux</t>
+        </is>
+      </c>
+      <c r="C311" t="n">
+        <v>0</v>
+      </c>
+      <c r="D311" t="n">
+        <v>54</v>
+      </c>
+      <c r="F311" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>TR</t>
+        </is>
+      </c>
+      <c r="C312" t="n">
+        <v>0</v>
+      </c>
+      <c r="D312" t="n">
+        <v>45</v>
+      </c>
+      <c r="F312" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>TR</t>
+        </is>
+      </c>
+      <c r="C313" t="n">
+        <v>0</v>
+      </c>
+      <c r="D313" t="n">
+        <v>45</v>
+      </c>
+      <c r="F313" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>HOY</t>
+        </is>
+      </c>
+      <c r="C314" t="n">
+        <v>0</v>
+      </c>
+      <c r="D314" t="n">
+        <v>32</v>
+      </c>
+      <c r="F314" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>313</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>HOY</t>
+        </is>
+      </c>
+      <c r="C315" t="n">
+        <v>0</v>
+      </c>
+      <c r="D315" t="n">
+        <v>32</v>
+      </c>
+      <c r="F315" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>314</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>fe</t>
+        </is>
+      </c>
+      <c r="C316" t="n">
+        <v>1</v>
+      </c>
+      <c r="D316" t="n">
+        <v>26</v>
+      </c>
+      <c r="F316" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -8836,7 +9273,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I293"/>
+  <dimension ref="A1:I316"/>
   <sheetViews>
     <sheetView topLeftCell="A168" workbookViewId="0">
       <selection activeCell="B182" sqref="B182:I182"/>
@@ -16012,6 +16449,259 @@
         <v>1</v>
       </c>
       <c r="G293" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>292</v>
+      </c>
+      <c r="C294" t="n">
+        <v>1</v>
+      </c>
+      <c r="G294" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>293</v>
+      </c>
+      <c r="C295" t="n">
+        <v>1</v>
+      </c>
+      <c r="G295" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>294</v>
+      </c>
+      <c r="C296" t="n">
+        <v>1</v>
+      </c>
+      <c r="G296" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>295</v>
+      </c>
+      <c r="C297" t="n">
+        <v>1</v>
+      </c>
+      <c r="G297" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>296</v>
+      </c>
+      <c r="C298" t="n">
+        <v>1</v>
+      </c>
+      <c r="G298" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>297</v>
+      </c>
+      <c r="C299" t="n">
+        <v>1</v>
+      </c>
+      <c r="G299" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>298</v>
+      </c>
+      <c r="C300" t="n">
+        <v>1</v>
+      </c>
+      <c r="G300" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>299</v>
+      </c>
+      <c r="C301" t="n">
+        <v>1</v>
+      </c>
+      <c r="G301" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>300</v>
+      </c>
+      <c r="C302" t="n">
+        <v>1</v>
+      </c>
+      <c r="G302" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>301</v>
+      </c>
+      <c r="C303" t="n">
+        <v>2</v>
+      </c>
+      <c r="G303" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>302</v>
+      </c>
+      <c r="C304" t="n">
+        <v>1</v>
+      </c>
+      <c r="G304" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>303</v>
+      </c>
+      <c r="C305" t="n">
+        <v>1</v>
+      </c>
+      <c r="G305" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>304</v>
+      </c>
+      <c r="C306" t="n">
+        <v>1</v>
+      </c>
+      <c r="G306" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>305</v>
+      </c>
+      <c r="C307" t="n">
+        <v>1</v>
+      </c>
+      <c r="G307" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>306</v>
+      </c>
+      <c r="C308" t="n">
+        <v>1</v>
+      </c>
+      <c r="G308" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>307</v>
+      </c>
+      <c r="C309" t="n">
+        <v>1</v>
+      </c>
+      <c r="G309" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>308</v>
+      </c>
+      <c r="C310" t="n">
+        <v>1</v>
+      </c>
+      <c r="G310" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>309</v>
+      </c>
+      <c r="C311" t="n">
+        <v>1</v>
+      </c>
+      <c r="G311" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>310</v>
+      </c>
+      <c r="C312" t="n">
+        <v>1</v>
+      </c>
+      <c r="G312" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>311</v>
+      </c>
+      <c r="C313" t="n">
+        <v>1</v>
+      </c>
+      <c r="G313" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>312</v>
+      </c>
+      <c r="C314" t="n">
+        <v>1</v>
+      </c>
+      <c r="G314" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>313</v>
+      </c>
+      <c r="C315" t="n">
+        <v>1</v>
+      </c>
+      <c r="G315" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>314</v>
+      </c>
+      <c r="C316" t="n">
+        <v>2</v>
+      </c>
+      <c r="G316" t="n">
         <v>100</v>
       </c>
     </row>
@@ -16026,7 +16716,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M293"/>
+  <dimension ref="A1:M316"/>
   <sheetViews>
     <sheetView topLeftCell="A168" workbookViewId="0">
       <selection activeCell="A182" sqref="A182"/>
@@ -23863,6 +24553,121 @@
     <row r="293">
       <c r="A293" t="n">
         <v>291</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -23876,7 +24681,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M293"/>
+  <dimension ref="A1:M316"/>
   <sheetViews>
     <sheetView topLeftCell="A164" workbookViewId="0">
       <selection activeCell="B182" sqref="B182:M182"/>
@@ -31850,6 +32655,121 @@
     <row r="293">
       <c r="A293" t="n">
         <v>291</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -31866,7 +32786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG293"/>
+  <dimension ref="A1:AG316"/>
   <sheetViews>
     <sheetView topLeftCell="A169" workbookViewId="0">
       <selection activeCell="F195" sqref="F195"/>
@@ -61533,6 +62453,2329 @@
       </c>
       <c r="AG293" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>292</v>
+      </c>
+      <c r="B294" t="n">
+        <v>1</v>
+      </c>
+      <c r="C294" t="n">
+        <v>1</v>
+      </c>
+      <c r="D294" t="n">
+        <v>1</v>
+      </c>
+      <c r="E294" t="n">
+        <v>1</v>
+      </c>
+      <c r="F294" t="n">
+        <v>1</v>
+      </c>
+      <c r="G294" t="n">
+        <v>1</v>
+      </c>
+      <c r="H294" t="n">
+        <v>1</v>
+      </c>
+      <c r="I294" t="n">
+        <v>1</v>
+      </c>
+      <c r="J294" t="n">
+        <v>1</v>
+      </c>
+      <c r="K294" t="n">
+        <v>1</v>
+      </c>
+      <c r="L294" t="n">
+        <v>1</v>
+      </c>
+      <c r="M294" t="n">
+        <v>1</v>
+      </c>
+      <c r="N294" t="n">
+        <v>11</v>
+      </c>
+      <c r="O294" t="n">
+        <v>1</v>
+      </c>
+      <c r="P294" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q294" t="n">
+        <v>1</v>
+      </c>
+      <c r="R294" t="n">
+        <v>1</v>
+      </c>
+      <c r="S294" t="n">
+        <v>1</v>
+      </c>
+      <c r="T294" t="n">
+        <v>1</v>
+      </c>
+      <c r="U294" t="n">
+        <v>11</v>
+      </c>
+      <c r="V294" t="n">
+        <v>1</v>
+      </c>
+      <c r="W294" t="n">
+        <v>1</v>
+      </c>
+      <c r="X294" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y294" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z294" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA294" t="n">
+        <v>11</v>
+      </c>
+      <c r="AB294" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC294" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD294" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE294" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF294" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG294" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="n">
+        <v>0</v>
+      </c>
+      <c r="C295" t="n">
+        <v>0</v>
+      </c>
+      <c r="D295" t="n">
+        <v>0</v>
+      </c>
+      <c r="E295" t="n">
+        <v>0</v>
+      </c>
+      <c r="F295" t="n">
+        <v>0</v>
+      </c>
+      <c r="G295" t="n">
+        <v>0</v>
+      </c>
+      <c r="H295" t="n">
+        <v>0</v>
+      </c>
+      <c r="I295" t="n">
+        <v>0</v>
+      </c>
+      <c r="J295" t="n">
+        <v>0</v>
+      </c>
+      <c r="K295" t="n">
+        <v>0</v>
+      </c>
+      <c r="L295" t="n">
+        <v>0</v>
+      </c>
+      <c r="M295" t="n">
+        <v>0</v>
+      </c>
+      <c r="N295" t="n">
+        <v>0</v>
+      </c>
+      <c r="O295" t="n">
+        <v>0</v>
+      </c>
+      <c r="P295" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q295" t="n">
+        <v>0</v>
+      </c>
+      <c r="R295" t="n">
+        <v>0</v>
+      </c>
+      <c r="S295" t="n">
+        <v>0</v>
+      </c>
+      <c r="T295" t="n">
+        <v>0</v>
+      </c>
+      <c r="U295" t="n">
+        <v>0</v>
+      </c>
+      <c r="V295" t="n">
+        <v>0</v>
+      </c>
+      <c r="W295" t="n">
+        <v>0</v>
+      </c>
+      <c r="X295" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y295" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z295" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA295" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB295" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC295" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD295" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE295" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF295" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG295" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="n">
+        <v>0</v>
+      </c>
+      <c r="C296" t="n">
+        <v>0</v>
+      </c>
+      <c r="D296" t="n">
+        <v>0</v>
+      </c>
+      <c r="E296" t="n">
+        <v>0</v>
+      </c>
+      <c r="F296" t="n">
+        <v>0</v>
+      </c>
+      <c r="G296" t="n">
+        <v>0</v>
+      </c>
+      <c r="H296" t="n">
+        <v>0</v>
+      </c>
+      <c r="I296" t="n">
+        <v>0</v>
+      </c>
+      <c r="J296" t="n">
+        <v>0</v>
+      </c>
+      <c r="K296" t="n">
+        <v>0</v>
+      </c>
+      <c r="L296" t="n">
+        <v>0</v>
+      </c>
+      <c r="M296" t="n">
+        <v>0</v>
+      </c>
+      <c r="N296" t="n">
+        <v>0</v>
+      </c>
+      <c r="O296" t="n">
+        <v>0</v>
+      </c>
+      <c r="P296" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q296" t="n">
+        <v>0</v>
+      </c>
+      <c r="R296" t="n">
+        <v>0</v>
+      </c>
+      <c r="S296" t="n">
+        <v>0</v>
+      </c>
+      <c r="T296" t="n">
+        <v>0</v>
+      </c>
+      <c r="U296" t="n">
+        <v>0</v>
+      </c>
+      <c r="V296" t="n">
+        <v>0</v>
+      </c>
+      <c r="W296" t="n">
+        <v>0</v>
+      </c>
+      <c r="X296" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y296" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z296" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA296" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB296" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC296" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD296" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE296" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF296" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG296" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="n">
+        <v>0</v>
+      </c>
+      <c r="C297" t="n">
+        <v>0</v>
+      </c>
+      <c r="D297" t="n">
+        <v>0</v>
+      </c>
+      <c r="E297" t="n">
+        <v>0</v>
+      </c>
+      <c r="F297" t="n">
+        <v>0</v>
+      </c>
+      <c r="G297" t="n">
+        <v>0</v>
+      </c>
+      <c r="H297" t="n">
+        <v>0</v>
+      </c>
+      <c r="I297" t="n">
+        <v>0</v>
+      </c>
+      <c r="J297" t="n">
+        <v>0</v>
+      </c>
+      <c r="K297" t="n">
+        <v>0</v>
+      </c>
+      <c r="L297" t="n">
+        <v>0</v>
+      </c>
+      <c r="M297" t="n">
+        <v>0</v>
+      </c>
+      <c r="N297" t="n">
+        <v>0</v>
+      </c>
+      <c r="O297" t="n">
+        <v>0</v>
+      </c>
+      <c r="P297" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q297" t="n">
+        <v>0</v>
+      </c>
+      <c r="R297" t="n">
+        <v>0</v>
+      </c>
+      <c r="S297" t="n">
+        <v>0</v>
+      </c>
+      <c r="T297" t="n">
+        <v>0</v>
+      </c>
+      <c r="U297" t="n">
+        <v>0</v>
+      </c>
+      <c r="V297" t="n">
+        <v>0</v>
+      </c>
+      <c r="W297" t="n">
+        <v>0</v>
+      </c>
+      <c r="X297" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y297" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z297" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA297" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB297" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC297" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD297" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE297" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF297" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG297" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="n">
+        <v>0</v>
+      </c>
+      <c r="C298" t="n">
+        <v>0</v>
+      </c>
+      <c r="D298" t="n">
+        <v>0</v>
+      </c>
+      <c r="E298" t="n">
+        <v>0</v>
+      </c>
+      <c r="F298" t="n">
+        <v>0</v>
+      </c>
+      <c r="G298" t="n">
+        <v>0</v>
+      </c>
+      <c r="H298" t="n">
+        <v>0</v>
+      </c>
+      <c r="I298" t="n">
+        <v>0</v>
+      </c>
+      <c r="J298" t="n">
+        <v>0</v>
+      </c>
+      <c r="K298" t="n">
+        <v>0</v>
+      </c>
+      <c r="L298" t="n">
+        <v>0</v>
+      </c>
+      <c r="M298" t="n">
+        <v>0</v>
+      </c>
+      <c r="N298" t="n">
+        <v>0</v>
+      </c>
+      <c r="O298" t="n">
+        <v>0</v>
+      </c>
+      <c r="P298" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q298" t="n">
+        <v>0</v>
+      </c>
+      <c r="R298" t="n">
+        <v>0</v>
+      </c>
+      <c r="S298" t="n">
+        <v>0</v>
+      </c>
+      <c r="T298" t="n">
+        <v>0</v>
+      </c>
+      <c r="U298" t="n">
+        <v>0</v>
+      </c>
+      <c r="V298" t="n">
+        <v>0</v>
+      </c>
+      <c r="W298" t="n">
+        <v>0</v>
+      </c>
+      <c r="X298" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y298" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z298" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA298" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB298" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC298" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD298" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE298" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF298" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG298" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="n">
+        <v>0</v>
+      </c>
+      <c r="C299" t="n">
+        <v>0</v>
+      </c>
+      <c r="D299" t="n">
+        <v>0</v>
+      </c>
+      <c r="E299" t="n">
+        <v>0</v>
+      </c>
+      <c r="F299" t="n">
+        <v>0</v>
+      </c>
+      <c r="G299" t="n">
+        <v>0</v>
+      </c>
+      <c r="H299" t="n">
+        <v>0</v>
+      </c>
+      <c r="I299" t="n">
+        <v>0</v>
+      </c>
+      <c r="J299" t="n">
+        <v>0</v>
+      </c>
+      <c r="K299" t="n">
+        <v>0</v>
+      </c>
+      <c r="L299" t="n">
+        <v>0</v>
+      </c>
+      <c r="M299" t="n">
+        <v>0</v>
+      </c>
+      <c r="N299" t="n">
+        <v>0</v>
+      </c>
+      <c r="O299" t="n">
+        <v>0</v>
+      </c>
+      <c r="P299" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q299" t="n">
+        <v>0</v>
+      </c>
+      <c r="R299" t="n">
+        <v>0</v>
+      </c>
+      <c r="S299" t="n">
+        <v>0</v>
+      </c>
+      <c r="T299" t="n">
+        <v>0</v>
+      </c>
+      <c r="U299" t="n">
+        <v>0</v>
+      </c>
+      <c r="V299" t="n">
+        <v>0</v>
+      </c>
+      <c r="W299" t="n">
+        <v>0</v>
+      </c>
+      <c r="X299" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y299" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z299" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA299" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB299" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC299" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD299" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE299" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF299" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG299" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="n">
+        <v>0</v>
+      </c>
+      <c r="C300" t="n">
+        <v>0</v>
+      </c>
+      <c r="D300" t="n">
+        <v>0</v>
+      </c>
+      <c r="E300" t="n">
+        <v>0</v>
+      </c>
+      <c r="F300" t="n">
+        <v>0</v>
+      </c>
+      <c r="G300" t="n">
+        <v>0</v>
+      </c>
+      <c r="H300" t="n">
+        <v>0</v>
+      </c>
+      <c r="I300" t="n">
+        <v>0</v>
+      </c>
+      <c r="J300" t="n">
+        <v>0</v>
+      </c>
+      <c r="K300" t="n">
+        <v>0</v>
+      </c>
+      <c r="L300" t="n">
+        <v>0</v>
+      </c>
+      <c r="M300" t="n">
+        <v>0</v>
+      </c>
+      <c r="N300" t="n">
+        <v>0</v>
+      </c>
+      <c r="O300" t="n">
+        <v>0</v>
+      </c>
+      <c r="P300" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q300" t="n">
+        <v>0</v>
+      </c>
+      <c r="R300" t="n">
+        <v>0</v>
+      </c>
+      <c r="S300" t="n">
+        <v>0</v>
+      </c>
+      <c r="T300" t="n">
+        <v>0</v>
+      </c>
+      <c r="U300" t="n">
+        <v>0</v>
+      </c>
+      <c r="V300" t="n">
+        <v>0</v>
+      </c>
+      <c r="W300" t="n">
+        <v>0</v>
+      </c>
+      <c r="X300" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y300" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z300" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA300" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB300" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC300" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD300" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE300" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF300" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG300" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="n">
+        <v>0</v>
+      </c>
+      <c r="C301" t="n">
+        <v>0</v>
+      </c>
+      <c r="D301" t="n">
+        <v>0</v>
+      </c>
+      <c r="E301" t="n">
+        <v>0</v>
+      </c>
+      <c r="F301" t="n">
+        <v>0</v>
+      </c>
+      <c r="G301" t="n">
+        <v>0</v>
+      </c>
+      <c r="H301" t="n">
+        <v>0</v>
+      </c>
+      <c r="I301" t="n">
+        <v>0</v>
+      </c>
+      <c r="J301" t="n">
+        <v>0</v>
+      </c>
+      <c r="K301" t="n">
+        <v>0</v>
+      </c>
+      <c r="L301" t="n">
+        <v>0</v>
+      </c>
+      <c r="M301" t="n">
+        <v>0</v>
+      </c>
+      <c r="N301" t="n">
+        <v>0</v>
+      </c>
+      <c r="O301" t="n">
+        <v>0</v>
+      </c>
+      <c r="P301" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q301" t="n">
+        <v>0</v>
+      </c>
+      <c r="R301" t="n">
+        <v>0</v>
+      </c>
+      <c r="S301" t="n">
+        <v>0</v>
+      </c>
+      <c r="T301" t="n">
+        <v>0</v>
+      </c>
+      <c r="U301" t="n">
+        <v>0</v>
+      </c>
+      <c r="V301" t="n">
+        <v>0</v>
+      </c>
+      <c r="W301" t="n">
+        <v>0</v>
+      </c>
+      <c r="X301" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y301" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z301" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA301" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB301" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC301" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD301" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE301" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF301" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG301" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>300</v>
+      </c>
+      <c r="B302" t="n">
+        <v>0</v>
+      </c>
+      <c r="C302" t="n">
+        <v>0</v>
+      </c>
+      <c r="D302" t="n">
+        <v>0</v>
+      </c>
+      <c r="E302" t="n">
+        <v>0</v>
+      </c>
+      <c r="F302" t="n">
+        <v>0</v>
+      </c>
+      <c r="G302" t="n">
+        <v>0</v>
+      </c>
+      <c r="H302" t="n">
+        <v>0</v>
+      </c>
+      <c r="I302" t="n">
+        <v>0</v>
+      </c>
+      <c r="J302" t="n">
+        <v>0</v>
+      </c>
+      <c r="K302" t="n">
+        <v>0</v>
+      </c>
+      <c r="L302" t="n">
+        <v>0</v>
+      </c>
+      <c r="M302" t="n">
+        <v>0</v>
+      </c>
+      <c r="N302" t="n">
+        <v>0</v>
+      </c>
+      <c r="O302" t="n">
+        <v>0</v>
+      </c>
+      <c r="P302" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q302" t="n">
+        <v>0</v>
+      </c>
+      <c r="R302" t="n">
+        <v>0</v>
+      </c>
+      <c r="S302" t="n">
+        <v>0</v>
+      </c>
+      <c r="T302" t="n">
+        <v>0</v>
+      </c>
+      <c r="U302" t="n">
+        <v>0</v>
+      </c>
+      <c r="V302" t="n">
+        <v>0</v>
+      </c>
+      <c r="W302" t="n">
+        <v>0</v>
+      </c>
+      <c r="X302" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y302" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z302" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA302" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB302" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC302" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD302" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE302" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF302" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG302" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="n">
+        <v>0</v>
+      </c>
+      <c r="C303" t="n">
+        <v>0</v>
+      </c>
+      <c r="D303" t="n">
+        <v>0</v>
+      </c>
+      <c r="E303" t="n">
+        <v>0</v>
+      </c>
+      <c r="F303" t="n">
+        <v>0</v>
+      </c>
+      <c r="G303" t="n">
+        <v>0</v>
+      </c>
+      <c r="H303" t="n">
+        <v>0</v>
+      </c>
+      <c r="I303" t="n">
+        <v>0</v>
+      </c>
+      <c r="J303" t="n">
+        <v>0</v>
+      </c>
+      <c r="K303" t="n">
+        <v>0</v>
+      </c>
+      <c r="L303" t="n">
+        <v>0</v>
+      </c>
+      <c r="M303" t="n">
+        <v>0</v>
+      </c>
+      <c r="N303" t="n">
+        <v>0</v>
+      </c>
+      <c r="O303" t="n">
+        <v>0</v>
+      </c>
+      <c r="P303" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q303" t="n">
+        <v>0</v>
+      </c>
+      <c r="R303" t="n">
+        <v>0</v>
+      </c>
+      <c r="S303" t="n">
+        <v>0</v>
+      </c>
+      <c r="T303" t="n">
+        <v>0</v>
+      </c>
+      <c r="U303" t="n">
+        <v>0</v>
+      </c>
+      <c r="V303" t="n">
+        <v>0</v>
+      </c>
+      <c r="W303" t="n">
+        <v>0</v>
+      </c>
+      <c r="X303" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y303" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z303" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA303" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB303" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC303" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD303" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE303" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF303" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG303" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="n">
+        <v>0</v>
+      </c>
+      <c r="C304" t="n">
+        <v>0</v>
+      </c>
+      <c r="D304" t="n">
+        <v>0</v>
+      </c>
+      <c r="E304" t="n">
+        <v>0</v>
+      </c>
+      <c r="F304" t="n">
+        <v>0</v>
+      </c>
+      <c r="G304" t="n">
+        <v>0</v>
+      </c>
+      <c r="H304" t="n">
+        <v>0</v>
+      </c>
+      <c r="I304" t="n">
+        <v>0</v>
+      </c>
+      <c r="J304" t="n">
+        <v>0</v>
+      </c>
+      <c r="K304" t="n">
+        <v>0</v>
+      </c>
+      <c r="L304" t="n">
+        <v>0</v>
+      </c>
+      <c r="M304" t="n">
+        <v>0</v>
+      </c>
+      <c r="N304" t="n">
+        <v>0</v>
+      </c>
+      <c r="O304" t="n">
+        <v>0</v>
+      </c>
+      <c r="P304" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q304" t="n">
+        <v>0</v>
+      </c>
+      <c r="R304" t="n">
+        <v>0</v>
+      </c>
+      <c r="S304" t="n">
+        <v>0</v>
+      </c>
+      <c r="T304" t="n">
+        <v>0</v>
+      </c>
+      <c r="U304" t="n">
+        <v>0</v>
+      </c>
+      <c r="V304" t="n">
+        <v>0</v>
+      </c>
+      <c r="W304" t="n">
+        <v>0</v>
+      </c>
+      <c r="X304" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y304" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z304" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA304" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB304" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC304" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD304" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE304" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF304" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG304" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="n">
+        <v>0</v>
+      </c>
+      <c r="C305" t="n">
+        <v>0</v>
+      </c>
+      <c r="D305" t="n">
+        <v>0</v>
+      </c>
+      <c r="E305" t="n">
+        <v>0</v>
+      </c>
+      <c r="F305" t="n">
+        <v>0</v>
+      </c>
+      <c r="G305" t="n">
+        <v>0</v>
+      </c>
+      <c r="H305" t="n">
+        <v>0</v>
+      </c>
+      <c r="I305" t="n">
+        <v>0</v>
+      </c>
+      <c r="J305" t="n">
+        <v>0</v>
+      </c>
+      <c r="K305" t="n">
+        <v>0</v>
+      </c>
+      <c r="L305" t="n">
+        <v>0</v>
+      </c>
+      <c r="M305" t="n">
+        <v>0</v>
+      </c>
+      <c r="N305" t="n">
+        <v>0</v>
+      </c>
+      <c r="O305" t="n">
+        <v>0</v>
+      </c>
+      <c r="P305" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q305" t="n">
+        <v>0</v>
+      </c>
+      <c r="R305" t="n">
+        <v>0</v>
+      </c>
+      <c r="S305" t="n">
+        <v>0</v>
+      </c>
+      <c r="T305" t="n">
+        <v>0</v>
+      </c>
+      <c r="U305" t="n">
+        <v>0</v>
+      </c>
+      <c r="V305" t="n">
+        <v>0</v>
+      </c>
+      <c r="W305" t="n">
+        <v>0</v>
+      </c>
+      <c r="X305" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y305" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG305" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="n">
+        <v>0</v>
+      </c>
+      <c r="C306" t="n">
+        <v>0</v>
+      </c>
+      <c r="D306" t="n">
+        <v>0</v>
+      </c>
+      <c r="E306" t="n">
+        <v>0</v>
+      </c>
+      <c r="F306" t="n">
+        <v>0</v>
+      </c>
+      <c r="G306" t="n">
+        <v>0</v>
+      </c>
+      <c r="H306" t="n">
+        <v>0</v>
+      </c>
+      <c r="I306" t="n">
+        <v>0</v>
+      </c>
+      <c r="J306" t="n">
+        <v>0</v>
+      </c>
+      <c r="K306" t="n">
+        <v>0</v>
+      </c>
+      <c r="L306" t="n">
+        <v>0</v>
+      </c>
+      <c r="M306" t="n">
+        <v>0</v>
+      </c>
+      <c r="N306" t="n">
+        <v>0</v>
+      </c>
+      <c r="O306" t="n">
+        <v>0</v>
+      </c>
+      <c r="P306" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q306" t="n">
+        <v>0</v>
+      </c>
+      <c r="R306" t="n">
+        <v>0</v>
+      </c>
+      <c r="S306" t="n">
+        <v>0</v>
+      </c>
+      <c r="T306" t="n">
+        <v>0</v>
+      </c>
+      <c r="U306" t="n">
+        <v>0</v>
+      </c>
+      <c r="V306" t="n">
+        <v>0</v>
+      </c>
+      <c r="W306" t="n">
+        <v>0</v>
+      </c>
+      <c r="X306" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y306" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z306" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA306" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB306" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC306" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD306" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE306" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF306" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG306" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="n">
+        <v>0</v>
+      </c>
+      <c r="C307" t="n">
+        <v>0</v>
+      </c>
+      <c r="D307" t="n">
+        <v>0</v>
+      </c>
+      <c r="E307" t="n">
+        <v>0</v>
+      </c>
+      <c r="F307" t="n">
+        <v>0</v>
+      </c>
+      <c r="G307" t="n">
+        <v>0</v>
+      </c>
+      <c r="H307" t="n">
+        <v>0</v>
+      </c>
+      <c r="I307" t="n">
+        <v>0</v>
+      </c>
+      <c r="J307" t="n">
+        <v>0</v>
+      </c>
+      <c r="K307" t="n">
+        <v>0</v>
+      </c>
+      <c r="L307" t="n">
+        <v>0</v>
+      </c>
+      <c r="M307" t="n">
+        <v>0</v>
+      </c>
+      <c r="N307" t="n">
+        <v>0</v>
+      </c>
+      <c r="O307" t="n">
+        <v>0</v>
+      </c>
+      <c r="P307" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q307" t="n">
+        <v>0</v>
+      </c>
+      <c r="R307" t="n">
+        <v>0</v>
+      </c>
+      <c r="S307" t="n">
+        <v>0</v>
+      </c>
+      <c r="T307" t="n">
+        <v>0</v>
+      </c>
+      <c r="U307" t="n">
+        <v>0</v>
+      </c>
+      <c r="V307" t="n">
+        <v>0</v>
+      </c>
+      <c r="W307" t="n">
+        <v>0</v>
+      </c>
+      <c r="X307" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y307" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z307" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA307" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB307" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC307" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD307" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE307" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF307" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG307" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="n">
+        <v>0</v>
+      </c>
+      <c r="C308" t="n">
+        <v>0</v>
+      </c>
+      <c r="D308" t="n">
+        <v>0</v>
+      </c>
+      <c r="E308" t="n">
+        <v>0</v>
+      </c>
+      <c r="F308" t="n">
+        <v>0</v>
+      </c>
+      <c r="G308" t="n">
+        <v>0</v>
+      </c>
+      <c r="H308" t="n">
+        <v>0</v>
+      </c>
+      <c r="I308" t="n">
+        <v>0</v>
+      </c>
+      <c r="J308" t="n">
+        <v>0</v>
+      </c>
+      <c r="K308" t="n">
+        <v>0</v>
+      </c>
+      <c r="L308" t="n">
+        <v>0</v>
+      </c>
+      <c r="M308" t="n">
+        <v>0</v>
+      </c>
+      <c r="N308" t="n">
+        <v>0</v>
+      </c>
+      <c r="O308" t="n">
+        <v>0</v>
+      </c>
+      <c r="P308" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q308" t="n">
+        <v>0</v>
+      </c>
+      <c r="R308" t="n">
+        <v>0</v>
+      </c>
+      <c r="S308" t="n">
+        <v>0</v>
+      </c>
+      <c r="T308" t="n">
+        <v>0</v>
+      </c>
+      <c r="U308" t="n">
+        <v>0</v>
+      </c>
+      <c r="V308" t="n">
+        <v>0</v>
+      </c>
+      <c r="W308" t="n">
+        <v>0</v>
+      </c>
+      <c r="X308" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y308" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z308" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA308" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB308" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC308" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD308" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE308" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF308" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG308" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="n">
+        <v>0</v>
+      </c>
+      <c r="C309" t="n">
+        <v>0</v>
+      </c>
+      <c r="D309" t="n">
+        <v>0</v>
+      </c>
+      <c r="E309" t="n">
+        <v>0</v>
+      </c>
+      <c r="F309" t="n">
+        <v>0</v>
+      </c>
+      <c r="G309" t="n">
+        <v>0</v>
+      </c>
+      <c r="H309" t="n">
+        <v>0</v>
+      </c>
+      <c r="I309" t="n">
+        <v>0</v>
+      </c>
+      <c r="J309" t="n">
+        <v>0</v>
+      </c>
+      <c r="K309" t="n">
+        <v>0</v>
+      </c>
+      <c r="L309" t="n">
+        <v>0</v>
+      </c>
+      <c r="M309" t="n">
+        <v>0</v>
+      </c>
+      <c r="N309" t="n">
+        <v>0</v>
+      </c>
+      <c r="O309" t="n">
+        <v>0</v>
+      </c>
+      <c r="P309" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q309" t="n">
+        <v>0</v>
+      </c>
+      <c r="R309" t="n">
+        <v>0</v>
+      </c>
+      <c r="S309" t="n">
+        <v>0</v>
+      </c>
+      <c r="T309" t="n">
+        <v>0</v>
+      </c>
+      <c r="U309" t="n">
+        <v>0</v>
+      </c>
+      <c r="V309" t="n">
+        <v>0</v>
+      </c>
+      <c r="W309" t="n">
+        <v>0</v>
+      </c>
+      <c r="X309" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y309" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z309" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA309" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB309" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC309" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD309" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE309" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF309" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG309" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="n">
+        <v>0</v>
+      </c>
+      <c r="C310" t="n">
+        <v>0</v>
+      </c>
+      <c r="D310" t="n">
+        <v>0</v>
+      </c>
+      <c r="E310" t="n">
+        <v>0</v>
+      </c>
+      <c r="F310" t="n">
+        <v>0</v>
+      </c>
+      <c r="G310" t="n">
+        <v>0</v>
+      </c>
+      <c r="H310" t="n">
+        <v>0</v>
+      </c>
+      <c r="I310" t="n">
+        <v>0</v>
+      </c>
+      <c r="J310" t="n">
+        <v>0</v>
+      </c>
+      <c r="K310" t="n">
+        <v>0</v>
+      </c>
+      <c r="L310" t="n">
+        <v>0</v>
+      </c>
+      <c r="M310" t="n">
+        <v>0</v>
+      </c>
+      <c r="N310" t="n">
+        <v>0</v>
+      </c>
+      <c r="O310" t="n">
+        <v>0</v>
+      </c>
+      <c r="P310" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q310" t="n">
+        <v>0</v>
+      </c>
+      <c r="R310" t="n">
+        <v>0</v>
+      </c>
+      <c r="S310" t="n">
+        <v>0</v>
+      </c>
+      <c r="T310" t="n">
+        <v>0</v>
+      </c>
+      <c r="U310" t="n">
+        <v>0</v>
+      </c>
+      <c r="V310" t="n">
+        <v>0</v>
+      </c>
+      <c r="W310" t="n">
+        <v>0</v>
+      </c>
+      <c r="X310" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y310" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z310" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA310" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB310" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC310" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD310" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE310" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF310" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG310" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="n">
+        <v>0</v>
+      </c>
+      <c r="C311" t="n">
+        <v>0</v>
+      </c>
+      <c r="D311" t="n">
+        <v>0</v>
+      </c>
+      <c r="E311" t="n">
+        <v>0</v>
+      </c>
+      <c r="F311" t="n">
+        <v>0</v>
+      </c>
+      <c r="G311" t="n">
+        <v>0</v>
+      </c>
+      <c r="H311" t="n">
+        <v>0</v>
+      </c>
+      <c r="I311" t="n">
+        <v>0</v>
+      </c>
+      <c r="J311" t="n">
+        <v>0</v>
+      </c>
+      <c r="K311" t="n">
+        <v>0</v>
+      </c>
+      <c r="L311" t="n">
+        <v>0</v>
+      </c>
+      <c r="M311" t="n">
+        <v>0</v>
+      </c>
+      <c r="N311" t="n">
+        <v>0</v>
+      </c>
+      <c r="O311" t="n">
+        <v>0</v>
+      </c>
+      <c r="P311" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q311" t="n">
+        <v>0</v>
+      </c>
+      <c r="R311" t="n">
+        <v>0</v>
+      </c>
+      <c r="S311" t="n">
+        <v>0</v>
+      </c>
+      <c r="T311" t="n">
+        <v>0</v>
+      </c>
+      <c r="U311" t="n">
+        <v>0</v>
+      </c>
+      <c r="V311" t="n">
+        <v>0</v>
+      </c>
+      <c r="W311" t="n">
+        <v>0</v>
+      </c>
+      <c r="X311" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y311" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z311" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA311" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB311" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC311" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD311" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE311" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF311" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG311" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="n">
+        <v>1</v>
+      </c>
+      <c r="C312" t="n">
+        <v>1</v>
+      </c>
+      <c r="D312" t="n">
+        <v>1</v>
+      </c>
+      <c r="E312" t="n">
+        <v>1</v>
+      </c>
+      <c r="F312" t="n">
+        <v>1</v>
+      </c>
+      <c r="G312" t="n">
+        <v>1</v>
+      </c>
+      <c r="H312" t="n">
+        <v>1</v>
+      </c>
+      <c r="I312" t="n">
+        <v>1</v>
+      </c>
+      <c r="J312" t="n">
+        <v>1</v>
+      </c>
+      <c r="K312" t="n">
+        <v>1</v>
+      </c>
+      <c r="L312" t="n">
+        <v>1</v>
+      </c>
+      <c r="M312" t="n">
+        <v>1</v>
+      </c>
+      <c r="N312" t="n">
+        <v>1</v>
+      </c>
+      <c r="O312" t="n">
+        <v>1</v>
+      </c>
+      <c r="P312" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q312" t="n">
+        <v>1</v>
+      </c>
+      <c r="R312" t="n">
+        <v>1</v>
+      </c>
+      <c r="S312" t="n">
+        <v>1</v>
+      </c>
+      <c r="T312" t="n">
+        <v>1</v>
+      </c>
+      <c r="U312" t="n">
+        <v>1</v>
+      </c>
+      <c r="V312" t="n">
+        <v>1</v>
+      </c>
+      <c r="W312" t="n">
+        <v>1</v>
+      </c>
+      <c r="X312" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y312" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z312" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA312" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB312" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC312" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD312" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE312" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF312" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG312" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="n">
+        <v>1</v>
+      </c>
+      <c r="C313" t="n">
+        <v>1</v>
+      </c>
+      <c r="D313" t="n">
+        <v>1</v>
+      </c>
+      <c r="E313" t="n">
+        <v>1</v>
+      </c>
+      <c r="F313" t="n">
+        <v>1</v>
+      </c>
+      <c r="G313" t="n">
+        <v>1</v>
+      </c>
+      <c r="H313" t="n">
+        <v>1</v>
+      </c>
+      <c r="I313" t="n">
+        <v>1</v>
+      </c>
+      <c r="J313" t="n">
+        <v>1</v>
+      </c>
+      <c r="K313" t="n">
+        <v>1</v>
+      </c>
+      <c r="L313" t="n">
+        <v>1</v>
+      </c>
+      <c r="M313" t="n">
+        <v>1</v>
+      </c>
+      <c r="N313" t="n">
+        <v>1</v>
+      </c>
+      <c r="O313" t="n">
+        <v>1</v>
+      </c>
+      <c r="P313" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q313" t="n">
+        <v>1</v>
+      </c>
+      <c r="R313" t="n">
+        <v>1</v>
+      </c>
+      <c r="S313" t="n">
+        <v>1</v>
+      </c>
+      <c r="T313" t="n">
+        <v>1</v>
+      </c>
+      <c r="U313" t="n">
+        <v>1</v>
+      </c>
+      <c r="V313" t="n">
+        <v>1</v>
+      </c>
+      <c r="W313" t="n">
+        <v>1</v>
+      </c>
+      <c r="X313" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y313" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z313" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA313" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB313" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC313" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD313" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE313" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF313" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG313" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="n">
+        <v>11</v>
+      </c>
+      <c r="C314" t="n">
+        <v>1</v>
+      </c>
+      <c r="D314" t="n">
+        <v>1</v>
+      </c>
+      <c r="E314" t="n">
+        <v>1</v>
+      </c>
+      <c r="F314" t="n">
+        <v>1</v>
+      </c>
+      <c r="G314" t="n">
+        <v>1</v>
+      </c>
+      <c r="H314" t="n">
+        <v>1</v>
+      </c>
+      <c r="I314" t="n">
+        <v>1</v>
+      </c>
+      <c r="J314" t="n">
+        <v>1</v>
+      </c>
+      <c r="K314" t="n">
+        <v>11</v>
+      </c>
+      <c r="L314" t="n">
+        <v>1</v>
+      </c>
+      <c r="M314" t="n">
+        <v>1</v>
+      </c>
+      <c r="N314" t="n">
+        <v>1</v>
+      </c>
+      <c r="O314" t="n">
+        <v>1</v>
+      </c>
+      <c r="P314" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q314" t="n">
+        <v>1</v>
+      </c>
+      <c r="R314" t="n">
+        <v>11</v>
+      </c>
+      <c r="S314" t="n">
+        <v>1</v>
+      </c>
+      <c r="T314" t="n">
+        <v>1</v>
+      </c>
+      <c r="U314" t="n">
+        <v>1</v>
+      </c>
+      <c r="V314" t="n">
+        <v>11</v>
+      </c>
+      <c r="W314" t="n">
+        <v>1</v>
+      </c>
+      <c r="X314" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y314" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z314" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA314" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB314" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC314" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD314" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE314" t="n">
+        <v>11</v>
+      </c>
+      <c r="AF314" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG314" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>313</v>
+      </c>
+      <c r="B315" t="n">
+        <v>1</v>
+      </c>
+      <c r="C315" t="n">
+        <v>1</v>
+      </c>
+      <c r="D315" t="n">
+        <v>1</v>
+      </c>
+      <c r="E315" t="n">
+        <v>1</v>
+      </c>
+      <c r="F315" t="n">
+        <v>1</v>
+      </c>
+      <c r="G315" t="n">
+        <v>1</v>
+      </c>
+      <c r="H315" t="n">
+        <v>1</v>
+      </c>
+      <c r="I315" t="n">
+        <v>1</v>
+      </c>
+      <c r="J315" t="n">
+        <v>1</v>
+      </c>
+      <c r="K315" t="n">
+        <v>11</v>
+      </c>
+      <c r="L315" t="n">
+        <v>1</v>
+      </c>
+      <c r="M315" t="n">
+        <v>1</v>
+      </c>
+      <c r="N315" t="n">
+        <v>1</v>
+      </c>
+      <c r="O315" t="n">
+        <v>1</v>
+      </c>
+      <c r="P315" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q315" t="n">
+        <v>1</v>
+      </c>
+      <c r="R315" t="n">
+        <v>1</v>
+      </c>
+      <c r="S315" t="n">
+        <v>1</v>
+      </c>
+      <c r="T315" t="n">
+        <v>1</v>
+      </c>
+      <c r="U315" t="n">
+        <v>1</v>
+      </c>
+      <c r="V315" t="n">
+        <v>11</v>
+      </c>
+      <c r="W315" t="n">
+        <v>1</v>
+      </c>
+      <c r="X315" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y315" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z315" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA315" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB315" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC315" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD315" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE315" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF315" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG315" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>314</v>
+      </c>
+      <c r="B316" t="n">
+        <v>1</v>
+      </c>
+      <c r="C316" t="n">
+        <v>1</v>
+      </c>
+      <c r="D316" t="n">
+        <v>1</v>
+      </c>
+      <c r="E316" t="n">
+        <v>1</v>
+      </c>
+      <c r="F316" t="n">
+        <v>1</v>
+      </c>
+      <c r="G316" t="n">
+        <v>1</v>
+      </c>
+      <c r="H316" t="n">
+        <v>1</v>
+      </c>
+      <c r="I316" t="n">
+        <v>1</v>
+      </c>
+      <c r="J316" t="n">
+        <v>1</v>
+      </c>
+      <c r="K316" t="n">
+        <v>1</v>
+      </c>
+      <c r="L316" t="n">
+        <v>1</v>
+      </c>
+      <c r="M316" t="n">
+        <v>1</v>
+      </c>
+      <c r="N316" t="n">
+        <v>1</v>
+      </c>
+      <c r="O316" t="n">
+        <v>1</v>
+      </c>
+      <c r="P316" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q316" t="n">
+        <v>1</v>
+      </c>
+      <c r="R316" t="n">
+        <v>1</v>
+      </c>
+      <c r="S316" t="n">
+        <v>1</v>
+      </c>
+      <c r="T316" t="n">
+        <v>1</v>
+      </c>
+      <c r="U316" t="n">
+        <v>1</v>
+      </c>
+      <c r="V316" t="n">
+        <v>1</v>
+      </c>
+      <c r="W316" t="n">
+        <v>1</v>
+      </c>
+      <c r="X316" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y316" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z316" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA316" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB316" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC316" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD316" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE316" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF316" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG316" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -61549,7 +64792,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J310"/>
+  <dimension ref="A1:J333"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
       <selection activeCell="F255" sqref="F255"/>
@@ -67378,7 +70621,6 @@
       <c r="A310" t="n">
         <v>291</v>
       </c>
-      <c r="C310" t="inlineStr"/>
       <c r="D310" t="n">
         <v>16</v>
       </c>
@@ -67387,6 +70629,329 @@
       </c>
       <c r="F310" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>292</v>
+      </c>
+      <c r="D311" t="n">
+        <v>16</v>
+      </c>
+      <c r="E311" t="n">
+        <v>100</v>
+      </c>
+      <c r="F311" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>293</v>
+      </c>
+      <c r="D312" t="n">
+        <v>16</v>
+      </c>
+      <c r="E312" t="n">
+        <v>100</v>
+      </c>
+      <c r="F312" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>294</v>
+      </c>
+      <c r="D313" t="n">
+        <v>8</v>
+      </c>
+      <c r="E313" t="n">
+        <v>50</v>
+      </c>
+      <c r="F313" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>295</v>
+      </c>
+      <c r="D314" t="n">
+        <v>12</v>
+      </c>
+      <c r="E314" t="n">
+        <v>75</v>
+      </c>
+      <c r="F314" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>296</v>
+      </c>
+      <c r="D315" t="n">
+        <v>1</v>
+      </c>
+      <c r="E315" t="n">
+        <v>1</v>
+      </c>
+      <c r="F315" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>297</v>
+      </c>
+      <c r="D316" t="n">
+        <v>1</v>
+      </c>
+      <c r="E316" t="n">
+        <v>1</v>
+      </c>
+      <c r="F316" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>298</v>
+      </c>
+      <c r="D317" t="n">
+        <v>1</v>
+      </c>
+      <c r="E317" t="n">
+        <v>1</v>
+      </c>
+      <c r="F317" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>299</v>
+      </c>
+      <c r="D318" t="n">
+        <v>1</v>
+      </c>
+      <c r="E318" t="n">
+        <v>1</v>
+      </c>
+      <c r="F318" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>300</v>
+      </c>
+      <c r="D319" t="n">
+        <v>1</v>
+      </c>
+      <c r="E319" t="n">
+        <v>1</v>
+      </c>
+      <c r="F319" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>301</v>
+      </c>
+      <c r="D320" t="n">
+        <v>1</v>
+      </c>
+      <c r="E320" t="n">
+        <v>1</v>
+      </c>
+      <c r="F320" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>302</v>
+      </c>
+      <c r="D321" t="n">
+        <v>1</v>
+      </c>
+      <c r="E321" t="n">
+        <v>1</v>
+      </c>
+      <c r="F321" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>303</v>
+      </c>
+      <c r="D322" t="n">
+        <v>1</v>
+      </c>
+      <c r="E322" t="n">
+        <v>1</v>
+      </c>
+      <c r="F322" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>304</v>
+      </c>
+      <c r="D323" t="n">
+        <v>1</v>
+      </c>
+      <c r="E323" t="n">
+        <v>1</v>
+      </c>
+      <c r="F323" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>305</v>
+      </c>
+      <c r="D324" t="n">
+        <v>1</v>
+      </c>
+      <c r="E324" t="n">
+        <v>1</v>
+      </c>
+      <c r="F324" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>306</v>
+      </c>
+      <c r="D325" t="n">
+        <v>1</v>
+      </c>
+      <c r="E325" t="n">
+        <v>1</v>
+      </c>
+      <c r="F325" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>307</v>
+      </c>
+      <c r="D326" t="n">
+        <v>1</v>
+      </c>
+      <c r="E326" t="n">
+        <v>1</v>
+      </c>
+      <c r="F326" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>308</v>
+      </c>
+      <c r="D327" t="n">
+        <v>1</v>
+      </c>
+      <c r="E327" t="n">
+        <v>1</v>
+      </c>
+      <c r="F327" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>309</v>
+      </c>
+      <c r="D328" t="n">
+        <v>1</v>
+      </c>
+      <c r="E328" t="n">
+        <v>1</v>
+      </c>
+      <c r="F328" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>310</v>
+      </c>
+      <c r="D329" t="n">
+        <v>16</v>
+      </c>
+      <c r="E329" t="n">
+        <v>100</v>
+      </c>
+      <c r="F329" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>311</v>
+      </c>
+      <c r="D330" t="n">
+        <v>12</v>
+      </c>
+      <c r="E330" t="n">
+        <v>78</v>
+      </c>
+      <c r="F330" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>312</v>
+      </c>
+      <c r="D331" t="n">
+        <v>16</v>
+      </c>
+      <c r="E331" t="n">
+        <v>100</v>
+      </c>
+      <c r="F331" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>313</v>
+      </c>
+      <c r="D332" t="n">
+        <v>9</v>
+      </c>
+      <c r="E332" t="n">
+        <v>79</v>
+      </c>
+      <c r="F332" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>314</v>
+      </c>
+      <c r="C333" t="inlineStr"/>
+      <c r="D333" t="n">
+        <v>9</v>
+      </c>
+      <c r="E333" t="n">
+        <v>79</v>
+      </c>
+      <c r="F333" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>